<commit_message>
fix: add minor fixes
</commit_message>
<xml_diff>
--- a/configuration-microservice/Admin_Panel_Features.xlsx
+++ b/configuration-microservice/Admin_Panel_Features.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms\Documents\Company\IDA-4\IDA\intelehealth-backend-service\configuration-microservice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1A5689-C642-48C7-9407-75B5D66FB75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E117A6-0CF1-42EC-9523-2C02C957600B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mst_patient_registration " sheetId="1" r:id="rId1"/>
+    <sheet name="mst_patient_registration" sheetId="1" r:id="rId1"/>
     <sheet name="mst_patient_vital" sheetId="2" r:id="rId2"/>
     <sheet name="mst_patient_visit_summary" sheetId="3" r:id="rId3"/>
     <sheet name="mst_dropdown_values" sheetId="4" r:id="rId4"/>
@@ -4540,7 +4540,7 @@
   </sheetPr>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -6864,7 +6864,7 @@
   </sheetPr>
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: update MySQL tables from Excel to set platform field if not already set
</commit_message>
<xml_diff>
--- a/configuration-microservice/Admin_Panel_Features.xlsx
+++ b/configuration-microservice/Admin_Panel_Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms\Documents\Company\IDA-4\IDA\intelehealth-backend-service\configuration-microservice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E117A6-0CF1-42EC-9523-2C02C957600B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D4E62A-31B8-49E7-BD56-75E65AC757F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mst_patient_registration" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="1406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3432" uniqueCount="1413">
   <si>
     <t>id</t>
   </si>
@@ -4250,6 +4250,27 @@
   </si>
   <si>
     <t>platform</t>
+  </si>
+  <si>
+    <t>Allow Duplicate PhoneNo And Email</t>
+  </si>
+  <si>
+    <t>Share Prescription</t>
+  </si>
+  <si>
+    <t>share_prescription</t>
+  </si>
+  <si>
+    <t>{"as": "", "bn": "", "en": "Prescription Share ", "gu": " પ્રિસ્ક્રિપ્શન શેર", "hi": "प्रिस्क्रिप्शन शेयर", "kn": "ಪ್ರಿಸ್ಕ್ರಿಪ್ಷನ್ ಹಂಚಿಕೆ", "mr": " प्रिस्क्रिप्शन शेअर", "or": "", "ru": "Рецепт Поделиться"}</t>
+  </si>
+  <si>
+    <t>Share Patient Visit Summary</t>
+  </si>
+  <si>
+    <t>share_patient_visit_summary</t>
+  </si>
+  <si>
+    <t>{"en": "Share Patient Visit Summary"}</t>
   </si>
 </sst>
 </file>
@@ -4259,7 +4280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4283,6 +4304,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4311,7 +4339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4320,6 +4348,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4540,7 +4570,7 @@
   </sheetPr>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I12" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -7913,10 +7943,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8620,6 +8650,26 @@
       </c>
       <c r="G32" s="5"/>
     </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>35</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45755.173900462964</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45764.237233796295</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F32" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -8627,6 +8677,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -25066,25 +25117,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="78.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="151.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="99" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -25519,6 +25568,82 @@
         <v>152</v>
       </c>
     </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>45757.430138888885</v>
+      </c>
+      <c r="I12" s="4">
+        <v>45768.4297337963</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D13" s="3">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>45757.430138888885</v>
+      </c>
+      <c r="I13" s="4">
+        <v>45768.4297337963</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{00000000-0002-0000-0800-000000000000}">

</xml_diff>